<commit_message>
Commiting some changes to mkcsv.py Expanding the reach of mkcsv to better include OCS controllers and notes. Also adding the ability to use cell formatting to add notes as Dave uses it to indicate various things.
</commit_message>
<xml_diff>
--- a/FLEX-TFLEX_Sim_June2015.xlsx
+++ b/FLEX-TFLEX_Sim_June2015.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/white/Repos/Dev/dbFlexControllers/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E75E6694-A0EA-B84C-85F2-8ED93387469D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1700" windowWidth="32000" windowHeight="19020"/>
+    <workbookView xWindow="25600" yWindow="14580" windowWidth="25600" windowHeight="14140" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TFLEX" sheetId="8" r:id="rId1"/>
     <sheet name="OCS" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="182">
   <si>
     <t>0010</t>
   </si>
@@ -621,13 +627,19 @@
   </si>
   <si>
     <t>881693723845</t>
+  </si>
+  <si>
+    <t>Iridium Phone</t>
+  </si>
+  <si>
+    <t>8988 1694 14000 461 473</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -679,6 +691,12 @@
       <b/>
       <sz val="10"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -743,7 +761,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -828,6 +846,15 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -838,11 +865,19 @@
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="3"/>
-    <cellStyle name="Normal 3" xfId="8"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1130,12 +1165,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11.33203125" style="7" customWidth="1"/>
     <col min="2" max="2" width="13" style="7" customWidth="1"/>
@@ -1146,7 +1181,7 @@
     <col min="7" max="16384" width="8.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="21" customFormat="1" ht="36" customHeight="1">
+    <row r="1" spans="1:6" s="21" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>32</v>
       </c>
@@ -1166,7 +1201,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="36" customHeight="1">
+    <row r="2" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>33</v>
       </c>
@@ -1186,7 +1221,7 @@
         <v>40334</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="36" customHeight="1">
+    <row r="3" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>37</v>
       </c>
@@ -1206,7 +1241,7 @@
         <v>40334</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="36" customHeight="1">
+    <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>41</v>
       </c>
@@ -1226,7 +1261,7 @@
         <v>40334</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="36" customHeight="1">
+    <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>45</v>
       </c>
@@ -1246,7 +1281,7 @@
         <v>40334</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="36" customHeight="1">
+    <row r="6" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>49</v>
       </c>
@@ -1266,7 +1301,7 @@
         <v>40815</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="36" customHeight="1">
+    <row r="7" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>53</v>
       </c>
@@ -1286,7 +1321,7 @@
         <v>40815</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="36" customHeight="1">
+    <row r="8" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>57</v>
       </c>
@@ -1306,7 +1341,7 @@
         <v>40815</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="36" customHeight="1">
+    <row r="9" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>61</v>
       </c>
@@ -1326,7 +1361,7 @@
         <v>40815</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="36" customHeight="1">
+    <row r="10" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>65</v>
       </c>
@@ -1346,7 +1381,7 @@
         <v>40969</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="36" customHeight="1">
+    <row r="11" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>69</v>
       </c>
@@ -1366,7 +1401,7 @@
         <v>40969</v>
       </c>
     </row>
-    <row r="12" spans="1:6" customFormat="1" ht="36" customHeight="1">
+    <row r="12" spans="1:6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
@@ -1386,7 +1421,7 @@
         <v>41424</v>
       </c>
     </row>
-    <row r="13" spans="1:6" customFormat="1" ht="36" customHeight="1">
+    <row r="13" spans="1:6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1406,7 +1441,7 @@
         <v>41424</v>
       </c>
     </row>
-    <row r="14" spans="1:6" customFormat="1" ht="36" customHeight="1">
+    <row r="14" spans="1:6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1426,7 +1461,7 @@
         <v>41424</v>
       </c>
     </row>
-    <row r="15" spans="1:6" customFormat="1" ht="36" customHeight="1">
+    <row r="15" spans="1:6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -1446,7 +1481,7 @@
         <v>41424</v>
       </c>
     </row>
-    <row r="16" spans="1:6" customFormat="1" ht="36" customHeight="1">
+    <row r="16" spans="1:6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1466,7 +1501,7 @@
         <v>41424</v>
       </c>
     </row>
-    <row r="17" spans="1:6" customFormat="1" ht="36" customHeight="1">
+    <row r="17" spans="1:6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1486,7 +1521,7 @@
         <v>41424</v>
       </c>
     </row>
-    <row r="18" spans="1:6" customFormat="1" ht="36" customHeight="1">
+    <row r="18" spans="1:6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1506,7 +1541,7 @@
         <v>41779</v>
       </c>
     </row>
-    <row r="19" spans="1:6" customFormat="1" ht="36" customHeight="1">
+    <row r="19" spans="1:6" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1526,7 +1561,7 @@
         <v>41779</v>
       </c>
     </row>
-    <row r="20" spans="1:6" customFormat="1" ht="35" customHeight="1">
+    <row r="20" spans="1:6" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>156</v>
       </c>
@@ -1546,7 +1581,7 @@
         <v>42297</v>
       </c>
     </row>
-    <row r="21" spans="1:6" customFormat="1" ht="35" customHeight="1">
+    <row r="21" spans="1:6" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>160</v>
       </c>
@@ -1566,7 +1601,7 @@
         <v>42297</v>
       </c>
     </row>
-    <row r="22" spans="1:6" customFormat="1" ht="35" customHeight="1">
+    <row r="22" spans="1:6" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>164</v>
       </c>
@@ -1586,7 +1621,7 @@
         <v>42297</v>
       </c>
     </row>
-    <row r="23" spans="1:6" customFormat="1" ht="35" customHeight="1">
+    <row r="23" spans="1:6" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>168</v>
       </c>
@@ -1606,7 +1641,7 @@
         <v>42297</v>
       </c>
     </row>
-    <row r="24" spans="1:6" customFormat="1" ht="35" customHeight="1">
+    <row r="24" spans="1:6" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>172</v>
       </c>
@@ -1626,7 +1661,7 @@
         <v>42324</v>
       </c>
     </row>
-    <row r="25" spans="1:6" customFormat="1" ht="35" customHeight="1">
+    <row r="25" spans="1:6" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>176</v>
       </c>
@@ -1646,7 +1681,7 @@
         <v>42324</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="13">
+    <row r="27" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="15" t="s">
         <v>73</v>
       </c>
@@ -1663,15 +1698,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="13" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.6640625" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" style="26" bestFit="1" customWidth="1"/>
@@ -1685,7 +1722,7 @@
     <col min="10" max="16384" width="12.5" style="26"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="23" customFormat="1">
+    <row r="1" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="22" t="s">
         <v>78</v>
       </c>
@@ -1714,7 +1751,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="25" t="s">
         <v>87</v>
       </c>
@@ -1740,7 +1777,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="25" t="s">
         <v>93</v>
       </c>
@@ -1760,7 +1797,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="25" t="s">
         <v>98</v>
       </c>
@@ -1792,7 +1829,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="25" t="s">
         <v>103</v>
       </c>
@@ -1824,7 +1861,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="25" t="s">
         <v>109</v>
       </c>
@@ -1838,7 +1875,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="25" t="s">
         <v>113</v>
       </c>
@@ -1870,7 +1907,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="25" t="s">
         <v>118</v>
       </c>
@@ -1890,7 +1927,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="25" t="s">
         <v>123</v>
       </c>
@@ -1910,7 +1947,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="25" t="s">
         <v>128</v>
       </c>
@@ -1936,7 +1973,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="25" t="s">
         <v>131</v>
       </c>
@@ -1965,7 +2002,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12" s="25" t="s">
         <v>135</v>
       </c>
@@ -1994,7 +2031,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13" s="25" t="s">
         <v>139</v>
       </c>
@@ -2023,7 +2060,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="25" t="s">
         <v>143</v>
       </c>
@@ -2052,7 +2089,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="25" t="s">
         <v>147</v>
       </c>
@@ -2081,7 +2118,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16" s="25" t="s">
         <v>151</v>
       </c>
@@ -2108,6 +2145,25 @@
       </c>
       <c r="I16" s="27" t="s">
         <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A17" s="31" t="s">
+        <v>180</v>
+      </c>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="H17" s="33">
+        <v>881641429998</v>
+      </c>
+      <c r="I17" s="33">
+        <v>881693429943</v>
       </c>
     </row>
   </sheetData>

</xml_diff>